<commit_message>
correzioni al self assessment
</commit_message>
<xml_diff>
--- a/report/Self-assessment-Mangini_Melluso.xlsx
+++ b/report/Self-assessment-Mangini_Melluso.xlsx
@@ -148,7 +148,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Nel progetto utilizziamo handlebars per disporre i risultati in maniera chiara. Utilizziamo delle card, in alcuni casi generate javascript in altri con Handlebars per mostrare ad esempio i risultati deller richerce sui film, ma ad esempio usiamo anche dei carousel e altri elementi per disporre gli elementi in maniera chiara. Utilizziamo delle funzioni asincrone, in modo che quando avvengono delle azioni sull'interfaccia, i dati vengano raccolti in maniera reattiva. Non sono stati utilizzati altri modi per comunicare tra il main server e i 2 server secondari. Il server comunicano correttamente l'uno con l'altro. Il main server Express invia le richieste agli altri 2 server che le elaborano, eseguono le operazioni e restituiscono i dati al main server. Per ogni azione all'interno della pagina corrisponde una funzione asincrona che esegue le richieste. Abbiamo usato Socket.IO per creare un sistema di chat in tempo reale. Ogni utente può accedere inserendo il nome e il ruolo, in modo che possano comunicare sia i fan che gli esperti. Sono presenti chat predefinite a seconda degli argomenti, altrimenti viene creata una room con un numero casuale o si può inserire direttamente il numero di una stanza. Una limitazione ad esempio è l'assenza di un sistema per memorizzare </t>
+    <t>Nel progetto utilizziamo handlebars per disporre i risultati in maniera chiara. Utilizziamo delle card, in alcuni casi generate con javascript in altri con Handlebars per mostrare ad esempio i risultati delle richerce sui film, ma ad esempio usiamo anche dei carousel e altri elementi per disporre gli elementi in maniera chiara. Utilizziamo delle funzioni asincrone, in modo che quando avvengono delle azioni sull'interfaccia, i dati vengano raccolti in maniera reattiva. Non sono stati utilizzati altri modi per comunicare tra il main server e i 2 server secondari. Il server comunicano correttamente l'uno con l'altro. Il main server Express invia le richieste agli altri 2 server che le elaborano, eseguono le operazioni e restituiscono i dati al main server. Per ogni azione all'interno della pagina corrisponde una funzione asincrona che esegue le richieste. Abbiamo usato Socket.IO per creare un sistema di chat in tempo reale. Ogni utente può accedere inserendo il nome e il ruolo, in modo che possano comunicare sia i fan che gli esperti. Sono presenti chat predefinite a seconda degli argomenti, altrimenti viene creata una room con un numero casuale o si può inserire direttamente il numero di una stanza. Una limitazione ad esempio è l'assenza di un sistema per memorizzare i messaggi.</t>
   </si>
   <si>
     <t>NodeJS Main Server  (IUM-TWEB)</t>
@@ -551,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -657,6 +657,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -1618,10 +1621,10 @@
       <c r="A75" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B75" s="31">
+      <c r="B75" s="43">
         <v>0.5</v>
       </c>
-      <c r="C75" s="31">
+      <c r="C75" s="43">
         <v>0.5</v>
       </c>
       <c r="D75" s="31">
@@ -1638,7 +1641,7 @@
       <c r="C76" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D76" s="43"/>
+      <c r="D76" s="44"/>
     </row>
     <row r="77" ht="16.5" customHeight="1">
       <c r="A77" s="37"/>

</xml_diff>